<commit_message>
There is a loop that makes bookings from excel rows, but not fully working
</commit_message>
<xml_diff>
--- a/uploads/excel.xlsx
+++ b/uploads/excel.xlsx
@@ -27,11 +27,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>name</t>
   </si>
   <si>
+    <t>12:45PM</t>
+  </si>
+  <si>
     <t>email</t>
   </si>
   <si>
@@ -41,28 +44,31 @@
     <t>endTime</t>
   </si>
   <si>
-    <t>Space</t>
-  </si>
-  <si>
-    <t>Reminder</t>
-  </si>
-  <si>
     <t>Huzaifa RAGHAV</t>
   </si>
   <si>
     <t>ragha59105@gapps.uwcsea.edu.sg</t>
   </si>
   <si>
-    <t>7 Nov 2017 12:45PM</t>
-  </si>
-  <si>
     <t>1:15PM</t>
   </si>
   <si>
     <t>Green Screen Room 1</t>
   </si>
   <si>
-    <t>12h</t>
+    <t>space</t>
+  </si>
+  <si>
+    <t>Carl CASTUERAS</t>
+  </si>
+  <si>
+    <t>cac59128@gapps.uwcsea.edu.sg</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>Green Screen Room 2</t>
   </si>
 </sst>
 </file>
@@ -109,8 +115,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -392,7 +398,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -402,10 +408,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -414,35 +420,53 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2">
+        <v>43046</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="1"/>
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2">
+        <v>43049</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
NEED spaceNameWithSpaces variable, or your_bookings and cancel e-mail does not work
</commit_message>
<xml_diff>
--- a/uploads/excel.xlsx
+++ b/uploads/excel.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffraghav/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffraghav/Desktop/booking_system_node_REAL/uploads/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4580" yWindow="8820" windowWidth="28800" windowHeight="16560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="16560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,14 +27,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>12:45PM</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
@@ -50,25 +47,31 @@
     <t>ragha59105@gapps.uwcsea.edu.sg</t>
   </si>
   <si>
-    <t>1:15PM</t>
-  </si>
-  <si>
     <t>Green Screen Room 1</t>
   </si>
   <si>
     <t>space</t>
   </si>
   <si>
-    <t>Carl CASTUERAS</t>
-  </si>
-  <si>
-    <t>cac59128@gapps.uwcsea.edu.sg</t>
-  </si>
-  <si>
     <t>day</t>
   </si>
   <si>
     <t>Green Screen Room 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reminder </t>
+  </si>
+  <si>
+    <t>12:45pm</t>
+  </si>
+  <si>
+    <t>1:15pm</t>
+  </si>
+  <si>
+    <t>12h</t>
+  </si>
+  <si>
+    <t>4h</t>
   </si>
 </sst>
 </file>
@@ -395,72 +398,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="C2" s="2">
         <v>43046</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2">
         <v>43049</v>
       </c>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>9</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created check for blank properties function
</commit_message>
<xml_diff>
--- a/uploads/excel.xlsx
+++ b/uploads/excel.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="16560" tabRatio="500"/>
+    <workbookView xWindow="4960" yWindow="6500" windowWidth="28800" windowHeight="16560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>name</t>
   </si>
@@ -53,15 +53,6 @@
     <t>space</t>
   </si>
   <si>
-    <t>day</t>
-  </si>
-  <si>
-    <t>Green Screen Room 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reminder </t>
-  </si>
-  <si>
     <t>12:45pm</t>
   </si>
   <si>
@@ -72,6 +63,12 @@
   </si>
   <si>
     <t>4h</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>reminder</t>
   </si>
 </sst>
 </file>
@@ -116,10 +113,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -398,84 +399,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
+      <c r="C1" s="4"/>
       <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
-        <v>10</v>
+      <c r="H1" s="4"/>
+      <c r="I1" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2">
+      <c r="D2" s="2">
         <v>43046</v>
       </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
-        <v>13</v>
+      <c r="I2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D3" s="2">
         <v>43049</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
       </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C4" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="G1:H1"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>

</xml_diff>